<commit_message>
1a correcion tablas de base de datos
</commit_message>
<xml_diff>
--- a/doc/base_sportfitness.xlsx
+++ b/doc/base_sportfitness.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tonito\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tonito\Desktop\SFitnessControl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1440F8-066B-423F-9774-A1924301D970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7289E9-30F5-4FEE-998E-B69D6141D216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13905" yWindow="840" windowWidth="21600" windowHeight="11385" xr2:uid="{900BD567-8373-419C-9BEF-5378AD0B5FB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{900BD567-8373-419C-9BEF-5378AD0B5FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>campos para crear tablas de base de datos de Sport Fitness</t>
   </si>
@@ -90,9 +90,6 @@
     <t>pwdadmin</t>
   </si>
   <si>
-    <t>IDusuario</t>
-  </si>
-  <si>
     <t>Idemail</t>
   </si>
   <si>
@@ -184,13 +181,22 @@
   </si>
   <si>
     <t>version office</t>
+  </si>
+  <si>
+    <t>Idusuario</t>
+  </si>
+  <si>
+    <t>activo( si, no)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,13 +219,37 @@
       <name val="Arial Black"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -231,16 +261,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -553,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9800C95F-3422-447D-9E61-4ADA2B755F27}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,11 +600,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -583,14 +618,14 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
+      <c r="A4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -601,7 +636,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -612,7 +647,7 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -620,10 +655,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -631,10 +666,10 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -642,7 +677,7 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -650,7 +685,7 @@
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -658,23 +693,23 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -682,15 +717,15 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -698,7 +733,7 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -706,100 +741,108 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>47</v>
-      </c>
       <c r="C23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>